<commit_message>
[karthik] Added some files to line estimate feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="approvalDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -216,10 +216,10 @@
     <t xml:space="preserve">work</t>
   </si>
   <si>
-    <t xml:space="preserve">AE456</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WIN456</t>
+    <t xml:space="preserve">AEN765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIN765</t>
   </si>
   <si>
     <t xml:space="preserve">Sq.metres</t>
@@ -237,7 +237,7 @@
     <t xml:space="preserve">admin</t>
   </si>
   <si>
-    <t xml:space="preserve">ADN456</t>
+    <t xml:space="preserve">ADN765</t>
   </si>
   <si>
     <t xml:space="preserve">technicalSanctionNumber</t>
@@ -252,7 +252,7 @@
     <t xml:space="preserve">technical</t>
   </si>
   <si>
-    <t xml:space="preserve">TSN456</t>
+    <t xml:space="preserve">TSN765</t>
   </si>
   <si>
     <t xml:space="preserve">Assistant Engineer</t>
@@ -421,12 +421,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,16 +525,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,11 +643,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.85204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,18 +697,21 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,13 +810,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,17 +861,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5864] resolved the create Spillover estimate feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="approvalDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -234,10 +234,16 @@
     <t xml:space="preserve">adminSanctionDate</t>
   </si>
   <si>
+    <t xml:space="preserve">administrativeSanctionAuthority</t>
+  </si>
+  <si>
     <t xml:space="preserve">admin</t>
   </si>
   <si>
     <t xml:space="preserve">ADN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commisioner</t>
   </si>
   <si>
     <t xml:space="preserve">technicalSanctionNumber</t>
@@ -387,11 +393,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -421,12 +427,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.0357142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,16 +530,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,11 +648,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.58673469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,13 +707,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,15 +813,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.3163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,16 +837,22 @@
       <c r="C1" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="D1" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="7" t="n">
+        <v>71</v>
+      </c>
+      <c r="C2" s="8" t="n">
         <v>42724</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -856,45 +873,44 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.2704081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>71</v>
+      <c r="B1" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="7" t="n">
+        <v>77</v>
+      </c>
+      <c r="C2" s="8" t="n">
         <v>42724</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-5858] Added some files for test
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
@@ -57,16 +57,16 @@
     <t xml:space="preserve">Forward to DEE</t>
   </si>
   <si>
-    <t xml:space="preserve">juniorAccountant</t>
+    <t xml:space="preserve">SuperIntendent</t>
   </si>
   <si>
     <t xml:space="preserve">ACCOUNTS</t>
   </si>
   <si>
-    <t xml:space="preserve">Junior Accountant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yash/ACC_IACC_1</t>
+    <t xml:space="preserve">Superintendent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K.Mohammed Juneed/ACC_Superintendent_2</t>
   </si>
   <si>
     <t xml:space="preserve">Forward to Accounts</t>
@@ -567,20 +567,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.5357142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.9234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -655,6 +655,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -679,18 +680,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3223,11 +3224,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5625,16 +5626,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6594,10 +6592,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6652,11 +6648,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5858] Scenario is done
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="130">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -81,12 +81,24 @@
     <t xml:space="preserve">Commissioner</t>
   </si>
   <si>
-    <t xml:space="preserve">S.Ravindra Babu ~ ADM_Commissioner_1</t>
+    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
   </si>
   <si>
     <t xml:space="preserve">Forward to commissioner</t>
   </si>
   <si>
+    <t xml:space="preserve">assis_Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to Engineer</t>
+  </si>
+  <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
@@ -403,9 +415,6 @@
   </si>
   <si>
     <t xml:space="preserve">TSN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assistant Engineer</t>
   </si>
 </sst>
 </file>
@@ -418,7 +427,7 @@
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -444,6 +453,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -508,7 +523,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -521,7 +536,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,7 +552,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -541,7 +564,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -570,17 +593,17 @@
   <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -654,6 +677,23 @@
         <v>19</v>
       </c>
       <c r="F4" s="2"/>
+    </row>
+    <row r="5" s="3" customFormat="true" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -680,18 +720,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,122 +739,122 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>31</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>33</v>
+      <c r="A2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="5" t="n">
         <v>48</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>42</v>
       </c>
+      <c r="I2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="M2" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="IX3" s="0"/>
       <c r="IY3" s="0"/>
@@ -1586,43 +1626,43 @@
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>40</v>
+        <v>67</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="IX4" s="0"/>
       <c r="IY4" s="0"/>
@@ -2394,43 +2434,43 @@
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="IX5" s="0"/>
       <c r="IY5" s="0"/>
@@ -3224,11 +3264,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3236,41 +3276,41 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="IX3" s="0"/>
       <c r="IY3" s="0"/>
@@ -4042,16 +4082,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>79</v>
+      <c r="D4" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="IX4" s="0"/>
       <c r="IY4" s="0"/>
@@ -4823,16 +4863,16 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="IX5" s="0"/>
       <c r="IY5" s="0"/>
@@ -5626,13 +5666,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5640,62 +5683,62 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="7" t="n">
+        <v>101</v>
+      </c>
+      <c r="B2" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>50000</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>50000</v>
@@ -5707,35 +5750,35 @@
         <v>1</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="7" t="n">
+        <v>106</v>
+      </c>
+      <c r="B3" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>200001</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>200001</v>
@@ -5747,10 +5790,10 @@
         <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -6000,27 +6043,27 @@
     </row>
     <row r="4" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="7" t="n">
+        <v>111</v>
+      </c>
+      <c r="B4" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>5000000</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>5000000</v>
@@ -6032,10 +6075,10 @@
         <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -6285,42 +6328,42 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="7" t="n">
+        <v>115</v>
+      </c>
+      <c r="B5" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>10000000</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -6592,8 +6635,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6601,27 +6646,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="9" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" s="11" t="n">
         <v>42724</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -6648,39 +6693,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>121</v>
+      <c r="B1" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="9" t="n">
+        <v>129</v>
+      </c>
+      <c r="C2" s="11" t="n">
         <v>42724</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>126</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-6000] completed new sewerage connection scenario
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="126">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -103,6 +103,24 @@
   </si>
   <si>
     <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeputyExecutiveEngineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.Radha Krishna/ENG_Dy. Executive Engineer_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Executive_engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Executive Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G.Raja Sekhar/ENG_Executive Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to executive engineer</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
@@ -398,11 +416,12 @@
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -420,12 +439,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -437,11 +450,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -499,49 +507,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,7 +521,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -557,7 +553,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -583,20 +579,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -688,7 +684,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" s="6" customFormat="true" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -698,11 +694,45 @@
       <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" s="3" customFormat="true" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -729,19 +759,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.719387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.3061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.9897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.1938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.234693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.6071428571429"/>
-    <col collapsed="false" hidden="false" max="254" min="12" style="1" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="255" style="0" width="11.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="254" min="12" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,209 +778,209 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>35</v>
       </c>
+      <c r="F1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="7" t="n">
+      <c r="A2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="5" t="n">
         <v>48</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>44</v>
+      <c r="E2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>52</v>
+        <v>57</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>42</v>
+        <v>67</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>42</v>
+      <c r="H5" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="9" t="n">
+        <v>75</v>
+      </c>
+      <c r="B6" s="7" t="n">
         <v>42887</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>42</v>
+      <c r="E6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -978,12 +1007,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="32.0204081632653"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="7.29081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,83 +1020,83 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1094,17 +1123,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.969387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="253" min="10" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="254" style="0" width="11.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="253" min="10" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,53 +1140,53 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="B2" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="n">
+      <c r="C2" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>50000</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>50000</v>
@@ -1169,27 +1197,27 @@
     </row>
     <row r="3" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="12" t="n">
+        <v>103</v>
+      </c>
+      <c r="B3" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="n">
+      <c r="C3" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>200001</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>200001</v>
@@ -1200,27 +1228,27 @@
     </row>
     <row r="4" s="1" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="12" t="n">
+        <v>107</v>
+      </c>
+      <c r="B4" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="n">
+      <c r="C4" s="9" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>5000000</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>5000000</v>
@@ -1231,64 +1259,64 @@
     </row>
     <row r="5" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="12" t="n">
+        <v>111</v>
+      </c>
+      <c r="B5" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>10000000</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="12" t="n">
+        <v>114</v>
+      </c>
+      <c r="B6" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C6" s="9" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>10000001</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1315,10 +1343,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2142857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1326,27 +1352,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="14" t="n">
+        <v>119</v>
+      </c>
+      <c r="C2" s="11" t="n">
         <v>42887</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1373,35 +1399,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>115</v>
+      <c r="B1" s="10" t="s">
+        <v>121</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="14" t="n">
+        <v>125</v>
+      </c>
+      <c r="C2" s="11" t="n">
         <v>42887</v>
       </c>
       <c r="D2" s="0" t="s">

</xml_diff>

<commit_message>
[PHOENIX-5850] Modified public works module
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
@@ -66,7 +66,7 @@
     <t xml:space="preserve">Superintendent</t>
   </si>
   <si>
-    <t xml:space="preserve">K.Mohammed Juneed/ACC_Superintendent_2</t>
+    <t xml:space="preserve">Mohammed Juneed/ACC_Superintendent_2</t>
   </si>
   <si>
     <t xml:space="preserve">Forward to Accounts</t>
@@ -582,17 +582,16 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.1836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -759,18 +758,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="254" min="12" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="254" min="12" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="255" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,12 +1007,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,16 +1123,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="253" min="10" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="253" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="254" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,8 +1344,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1399,11 +1402,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0051020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-6000] changes in excel sheet
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
@@ -81,7 +81,7 @@
     <t xml:space="preserve">Commissioner</t>
   </si>
   <si>
-    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
+    <t xml:space="preserve">Ravindra Babu/ADM_Commissioner_1</t>
   </si>
   <si>
     <t xml:space="preserve">Forward to commissioner</t>
@@ -582,16 +582,16 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.4489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.6989795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -758,17 +758,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.1326530612245"/>
     <col collapsed="false" hidden="false" max="254" min="12" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="1025" min="255" style="0" width="8.50510204081633"/>
   </cols>
@@ -1007,12 +1007,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,16 +1123,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="253" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="253" min="10" style="0" width="7.4234693877551"/>
     <col collapsed="false" hidden="false" max="1025" min="254" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -1345,8 +1345,8 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.4591836734694"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -1402,10 +1402,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7908163265306"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5850] Refactoring the code
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/lineEstimateTestData.xlsx
@@ -81,7 +81,7 @@
     <t xml:space="preserve">Commissioner</t>
   </si>
   <si>
-    <t xml:space="preserve">Ravindra Babu/ADM_Commissioner_1</t>
+    <t xml:space="preserve">Ravindra Babu/ADM_Commissioner_2</t>
   </si>
   <si>
     <t xml:space="preserve">Forward to commissioner</t>
@@ -587,11 +587,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -758,19 +759,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="26.7295918367347"/>
     <col collapsed="false" hidden="false" max="254" min="12" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="255" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="255" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,12 +1008,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,17 +1123,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="253" min="10" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="254" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="253" min="10" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="254" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,10 +1344,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1402,10 +1402,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>